<commit_message>
added jira handler and reports
</commit_message>
<xml_diff>
--- a/Final Project Part 2 (API)/test casess api project(part 2).xlsx
+++ b/Final Project Part 2 (API)/test casess api project(part 2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majdh\OneDrive\שולחן העבודה\Automation_bootcamp\Final Project Part 2 (API)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255F3326-25BD-4E0E-AFB6-567A6A98C703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD095B2-F213-40F7-991E-19AF7C8C84F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6DB08689-E348-4E0B-8AED-3F8E8057D764}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="109">
   <si>
     <t>Name of the test case</t>
   </si>
@@ -540,6 +540,9 @@
     <t>{
     "detail": "Retweets for tweet id = 1349129669258448897 not found"
 }</t>
+  </si>
+  <si>
+    <t>לכתוב יוזנייםת איידיי ת ספיציפים</t>
   </si>
 </sst>
 </file>
@@ -987,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D84E9B10-6DEB-4A0D-98B6-D1464F09588B}">
   <dimension ref="A1:C310"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E265" sqref="E265"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1174,6 +1177,9 @@
       <c r="B33" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="C33" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="34" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">

</xml_diff>